<commit_message>
Update output directory fix
</commit_message>
<xml_diff>
--- a/principal/src/main/resources/Output/Jaclupan_LR-2024.xlsx
+++ b/principal/src/main/resources/Output/Jaclupan_LR-2024.xlsx
@@ -747,7 +747,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -983,7 +983,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1952,7 +1951,7 @@
       <c r="E12" s="27"/>
     </row>
     <row r="13">
-      <c r="B13" t="s" s="97">
+      <c r="B13" t="s" s="0">
         <v>44</v>
       </c>
       <c r="C13" t="s" s="0">
@@ -1966,7 +1965,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="B14" t="s" s="97">
+      <c r="B14" t="s" s="0">
         <v>47</v>
       </c>
       <c r="C14" t="s" s="0">
@@ -1980,7 +1979,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="B15" t="s" s="97">
+      <c r="B15" t="s" s="0">
         <v>47</v>
       </c>
       <c r="C15" t="s" s="0">
@@ -1990,7 +1989,7 @@
         <v>49</v>
       </c>
       <c r="E15" t="n" s="0">
-        <v>3500.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="25" customHeight="1" x14ac:dyDescent="0.5">

</xml_diff>